<commit_message>
added missing data (now 10 persons)
</commit_message>
<xml_diff>
--- a/Wahrnehmungsstudie/Wahrnehmungsstudie.xlsx
+++ b/Wahrnehmungsstudie/Wahrnehmungsstudie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ericm\iCloudDrive\Dokumente\TU Dresden\Semester 3\Akustik NF\SoundDesign\Wahrnehmungsstudie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\Eric\TU Dresden\Semester 3\SoundDesign\WorkSpace\SoundDesignProject\Wahrnehmungsstudie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{AC228FA4-E236-46D7-B6E5-5011A8091F5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571236F9-75EF-49C2-9060-13250D956A60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" tabRatio="746"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" tabRatio="746" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Wahrnehmungsstudie" sheetId="1" r:id="rId1"/>
@@ -30,13 +30,22 @@
   <definedNames>
     <definedName name="Wahrnehmungsstudie" localSheetId="0">Wahrnehmungsstudie!$A$1:$DI$9</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="Wahrnehmungsstudie" type="6" refreshedVersion="7" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="Wahrnehmungsstudie" type="6" refreshedVersion="7" background="1" saveData="1">
     <textPr sourceFile="C:\Users\ericm\Downloads\Wahrnehmungsstudie.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="113">
         <textField/>
@@ -497,7 +506,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1191,25 +1200,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3.7777777777777777</c:v>
+                  <c:v>3.4545454545454546</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.5555555555555554</c:v>
+                  <c:v>2.3636363636363638</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.1111111111111112</c:v>
+                  <c:v>2.7272727272727271</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.7777777777777777</c:v>
+                  <c:v>1.6363636363636362</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.8888888888888888</c:v>
+                  <c:v>1.8181818181818181</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.4444444444444446</c:v>
+                  <c:v>1.4545454545454546</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3333333333333335</c:v>
+                  <c:v>1.2727272727272729</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1550,16 +1559,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2.125</c:v>
+                  <c:v>2.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.75</c:v>
+                  <c:v>0.79999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.875</c:v>
+                  <c:v>2.9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.25</c:v>
+                  <c:v>4.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1957,10 +1966,10 @@
                   <c:v>Motor 7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Motor 4</c:v>
+                  <c:v>Motor 6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Motor 6</c:v>
+                  <c:v>Motor 4</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Motor 5</c:v>
@@ -1981,34 +1990,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>3.25</c:v>
+                  <c:v>3.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.125</c:v>
+                  <c:v>3.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.375</c:v>
+                  <c:v>2.2000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.875</c:v>
+                  <c:v>1.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.75</c:v>
+                  <c:v>1.7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.75</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.625</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.5</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.625</c:v>
+                  <c:v>2.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2348,28 +2357,28 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.75</c:v>
+                  <c:v>2.9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.25</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.625</c:v>
+                  <c:v>1.7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.5</c:v>
+                  <c:v>1.4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5</c:v>
+                  <c:v>1.4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.375</c:v>
+                  <c:v>1.4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.375</c:v>
+                  <c:v>1.3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.125</c:v>
+                  <c:v>1.1000000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2710,25 +2719,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3.7777777777777777</c:v>
+                  <c:v>3.9090909090909092</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.1111111111111112</c:v>
+                  <c:v>3.1818181818181817</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.8888888888888888</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.8888888888888888</c:v>
+                  <c:v>1.9090909090909092</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.5555555555555554</c:v>
+                  <c:v>2.5454545454545454</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.1111111111111112</c:v>
+                  <c:v>2.1818181818181817</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.5555555555555554</c:v>
+                  <c:v>1.7272727272727271</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3063,25 +3072,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3.6666666666666665</c:v>
+                  <c:v>3.7272727272727271</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.2222222222222223</c:v>
+                  <c:v>3.3636363636363638</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.4444444444444446</c:v>
+                  <c:v>3.5454545454545454</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.3333333333333335</c:v>
+                  <c:v>2.2727272727272729</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.4444444444444446</c:v>
+                  <c:v>2.4545454545454546</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.1111111111111112</c:v>
+                  <c:v>2.2727272727272729</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>2.0909090909090908</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3449,25 +3458,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3.3333333333333335</c:v>
+                  <c:v>3.6363636363636362</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.6666666666666665</c:v>
+                  <c:v>2.8181818181818183</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.7777777777777777</c:v>
+                  <c:v>2.9090909090909092</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.7777777777777777</c:v>
+                  <c:v>1.8181818181818183</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.2222222222222223</c:v>
+                  <c:v>2.1818181818181817</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.1111111111111112</c:v>
+                  <c:v>2.1818181818181817</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.4444444444444446</c:v>
+                  <c:v>2.4545454545454546</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3835,25 +3844,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>2.2222222222222223</c:v>
+                  <c:v>2.0909090909090908</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.3333333333333335</c:v>
+                  <c:v>3.2727272727272729</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>3.9090909090909092</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.2222222222222223</c:v>
+                  <c:v>3.0909090909090908</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.2222222222222223</c:v>
+                  <c:v>2.2727272727272729</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.4444444444444446</c:v>
+                  <c:v>2.5454545454545454</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3</c:v>
+                  <c:v>3.0909090909090908</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4221,25 +4230,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>3.9090909090909092</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.1111111111111112</c:v>
+                  <c:v>3.1818181818181817</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.3333333333333335</c:v>
+                  <c:v>3.2727272727272729</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.25</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.6666666666666667</c:v>
+                  <c:v>1.7272727272727273</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.3333333333333335</c:v>
+                  <c:v>2.2727272727272729</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.1111111111111112</c:v>
+                  <c:v>2.0909090909090908</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4607,25 +4616,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3.7777777777777777</c:v>
+                  <c:v>3.7272727272727271</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.4444444444444446</c:v>
+                  <c:v>3.3636363636363638</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.2222222222222223</c:v>
+                  <c:v>3.0909090909090908</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.3333333333333335</c:v>
+                  <c:v>2.4545454545454546</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.4444444444444446</c:v>
+                  <c:v>2.4545454545454546</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.1111111111111112</c:v>
+                  <c:v>2.1818181818181817</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.1111111111111112</c:v>
+                  <c:v>2.1818181818181817</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4993,25 +5002,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3.4444444444444446</c:v>
+                  <c:v>3.3636363636363638</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.2222222222222223</c:v>
+                  <c:v>3.1818181818181817</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.5555555555555554</c:v>
+                  <c:v>3.3636363636363638</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.2222222222222223</c:v>
+                  <c:v>2.1818181818181817</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.4444444444444446</c:v>
+                  <c:v>3.4545454545454546</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.3333333333333335</c:v>
+                  <c:v>1.3636363636363638</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.5555555555555554</c:v>
+                  <c:v>1.7272727272727271</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5379,25 +5388,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3.8888888888888888</c:v>
+                  <c:v>3.9090909090909092</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.2222222222222223</c:v>
+                  <c:v>3.3636363636363638</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.8888888888888888</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.7777777777777777</c:v>
+                  <c:v>1.8181818181818183</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.6666666666666665</c:v>
+                  <c:v>2.7272727272727271</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5555555555555554</c:v>
+                  <c:v>1.6363636363636362</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3333333333333335</c:v>
+                  <c:v>1.5454545454545454</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12456,7 +12465,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Wahrnehmungsstudie" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Wahrnehmungsstudie" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -15043,11 +15052,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DI9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17728,11 +17737,11 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:R12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="B4:R14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C10"/>
+      <selection activeCell="L13" sqref="L13:R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17743,7 +17752,7 @@
       </c>
       <c r="C4">
         <f>AVERAGE(L:L)</f>
-        <v>3.8888888888888888</v>
+        <v>3.9090909090909092</v>
       </c>
       <c r="L4">
         <v>4</v>
@@ -17773,7 +17782,7 @@
       </c>
       <c r="C5">
         <f>AVERAGE(O:O)</f>
-        <v>3.2222222222222223</v>
+        <v>3.3636363636363638</v>
       </c>
       <c r="L5">
         <v>4</v>
@@ -17803,7 +17812,7 @@
       </c>
       <c r="C6">
         <f>AVERAGE(M:M)</f>
-        <v>2.8888888888888888</v>
+        <v>3</v>
       </c>
       <c r="L6">
         <v>4</v>
@@ -17833,7 +17842,7 @@
       </c>
       <c r="C7">
         <f>5 - AVERAGE(R:R)</f>
-        <v>1.7777777777777777</v>
+        <v>1.8181818181818183</v>
       </c>
       <c r="L7">
         <v>5</v>
@@ -17863,7 +17872,7 @@
       </c>
       <c r="C8">
         <f>AVERAGE(N:N)</f>
-        <v>2.6666666666666665</v>
+        <v>2.7272727272727271</v>
       </c>
       <c r="L8">
         <v>4</v>
@@ -17893,7 +17902,7 @@
       </c>
       <c r="C9">
         <f>5 - AVERAGE(P:P)</f>
-        <v>1.5555555555555554</v>
+        <v>1.6363636363636362</v>
       </c>
       <c r="L9">
         <v>4</v>
@@ -17923,7 +17932,7 @@
       </c>
       <c r="C10">
         <f>5 - AVERAGE(Q:Q)</f>
-        <v>1.3333333333333335</v>
+        <v>1.5454545454545454</v>
       </c>
       <c r="L10">
         <v>2</v>
@@ -17991,6 +18000,52 @@
       </c>
       <c r="R12">
         <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="L13">
+        <v>4</v>
+      </c>
+      <c r="M13">
+        <v>4</v>
+      </c>
+      <c r="N13">
+        <v>3</v>
+      </c>
+      <c r="O13">
+        <v>4</v>
+      </c>
+      <c r="P13">
+        <v>4</v>
+      </c>
+      <c r="Q13">
+        <v>3</v>
+      </c>
+      <c r="R13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="L14">
+        <v>4</v>
+      </c>
+      <c r="M14">
+        <v>3</v>
+      </c>
+      <c r="N14">
+        <v>3</v>
+      </c>
+      <c r="O14">
+        <v>4</v>
+      </c>
+      <c r="P14">
+        <v>2</v>
+      </c>
+      <c r="Q14">
+        <v>2</v>
+      </c>
+      <c r="R14">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -18000,11 +18055,11 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:J12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="B5:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="I13" sqref="I13:J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18015,7 +18070,7 @@
       </c>
       <c r="C5">
         <f>5 - AVERAGE(I:I)</f>
-        <v>2.125</v>
+        <v>2.1</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -18030,7 +18085,7 @@
       </c>
       <c r="C6">
         <f>5 - AVERAGE(J:J)</f>
-        <v>0.75</v>
+        <v>0.79999999999999982</v>
       </c>
       <c r="I6">
         <v>4</v>
@@ -18045,7 +18100,7 @@
       </c>
       <c r="C7">
         <f>AVERAGE(I:I)</f>
-        <v>2.875</v>
+        <v>2.9</v>
       </c>
       <c r="I7">
         <v>4</v>
@@ -18060,7 +18115,7 @@
       </c>
       <c r="C8">
         <f>AVERAGE(J:J)</f>
-        <v>4.25</v>
+        <v>4.2</v>
       </c>
       <c r="I8">
         <v>3</v>
@@ -18099,6 +18154,22 @@
       </c>
       <c r="J12">
         <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I13">
+        <v>3</v>
+      </c>
+      <c r="J13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I14">
+        <v>3</v>
+      </c>
+      <c r="J14">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -18108,11 +18179,11 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="B4:P14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18162,7 +18233,7 @@
       </c>
       <c r="C5">
         <f>AVERAGE(M:M)</f>
-        <v>3.25</v>
+        <v>3.4</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -18201,7 +18272,7 @@
       </c>
       <c r="C6">
         <f>AVERAGE(N:N)</f>
-        <v>3.125</v>
+        <v>3.1</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -18279,7 +18350,7 @@
       </c>
       <c r="C8">
         <f>AVERAGE(F:F)</f>
-        <v>2.375</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F8">
         <v>5</v>
@@ -18318,7 +18389,7 @@
       </c>
       <c r="C9">
         <f>AVERAGE(L:L)</f>
-        <v>1.875</v>
+        <v>1.7</v>
       </c>
       <c r="F9">
         <v>3</v>
@@ -18353,11 +18424,11 @@
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C10">
-        <f>AVERAGE(I:I)</f>
-        <v>1.75</v>
+        <f>AVERAGE(K:K)</f>
+        <v>1.7</v>
       </c>
       <c r="F10">
         <v>2</v>
@@ -18392,11 +18463,11 @@
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C11">
-        <f>AVERAGE(K:K)</f>
-        <v>1.75</v>
+        <f>AVERAGE(I:I)</f>
+        <v>1.6</v>
       </c>
       <c r="F11">
         <v>3</v>
@@ -18435,7 +18506,37 @@
       </c>
       <c r="C12">
         <f>AVERAGE(J:J)</f>
-        <v>1.625</v>
+        <v>1.6</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>2</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>4</v>
+      </c>
+      <c r="N12">
+        <v>3</v>
+      </c>
+      <c r="P12">
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.3">
@@ -18444,7 +18545,37 @@
       </c>
       <c r="C13">
         <f>AVERAGE(H:H)</f>
-        <v>1.5</v>
+        <v>1.6</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>2</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>4</v>
+      </c>
+      <c r="N13">
+        <v>3</v>
+      </c>
+      <c r="P13">
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.3">
@@ -18452,8 +18583,8 @@
         <v>110</v>
       </c>
       <c r="C14">
-        <f>AVERAGE(P4:P11)</f>
-        <v>2.625</v>
+        <f>AVERAGE(P:P)</f>
+        <v>2.8</v>
       </c>
     </row>
   </sheetData>
@@ -18467,11 +18598,11 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="B4:N13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18553,7 +18684,7 @@
       </c>
       <c r="C6">
         <f>AVERAGE(M:M)</f>
-        <v>2.75</v>
+        <v>2.9</v>
       </c>
       <c r="F6">
         <v>2</v>
@@ -18589,7 +18720,7 @@
       </c>
       <c r="C7">
         <f>AVERAGE(F:F)</f>
-        <v>2.25</v>
+        <v>2</v>
       </c>
       <c r="F7">
         <v>4</v>
@@ -18625,7 +18756,7 @@
       </c>
       <c r="C8">
         <f>AVERAGE(G:G)</f>
-        <v>1.625</v>
+        <v>1.7</v>
       </c>
       <c r="F8">
         <v>4</v>
@@ -18661,7 +18792,7 @@
       </c>
       <c r="C9">
         <f>AVERAGE(K:K)</f>
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="F9">
         <v>2</v>
@@ -18697,7 +18828,7 @@
       </c>
       <c r="C10">
         <f>AVERAGE(L:L)</f>
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -18733,7 +18864,7 @@
       </c>
       <c r="C11">
         <f>AVERAGE(H:H)</f>
-        <v>1.375</v>
+        <v>1.4</v>
       </c>
       <c r="F11">
         <v>2</v>
@@ -18769,7 +18900,34 @@
       </c>
       <c r="C12">
         <f>AVERAGE(J:J)</f>
-        <v>1.375</v>
+        <v>1.3</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>3</v>
+      </c>
+      <c r="N12">
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
@@ -18778,7 +18936,34 @@
       </c>
       <c r="C13">
         <f>AVERAGE(I:I)</f>
-        <v>1.125</v>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>4</v>
+      </c>
+      <c r="N13">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -18791,11 +18976,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:R12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B4:R14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+      <selection activeCell="M17" sqref="M16:M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18809,7 +18994,7 @@
       </c>
       <c r="C4">
         <f>AVERAGE(L:L)</f>
-        <v>3.7777777777777777</v>
+        <v>3.4545454545454546</v>
       </c>
       <c r="L4">
         <v>5</v>
@@ -18839,7 +19024,7 @@
       </c>
       <c r="C5">
         <f>AVERAGE(O:O)</f>
-        <v>2.5555555555555554</v>
+        <v>2.3636363636363638</v>
       </c>
       <c r="L5">
         <v>3</v>
@@ -18869,7 +19054,7 @@
       </c>
       <c r="C6">
         <f>AVERAGE(M:M)</f>
-        <v>3.1111111111111112</v>
+        <v>2.7272727272727271</v>
       </c>
       <c r="L6">
         <v>4</v>
@@ -18899,7 +19084,7 @@
       </c>
       <c r="C7">
         <f>5 - AVERAGE(R:R)</f>
-        <v>1.7777777777777777</v>
+        <v>1.6363636363636362</v>
       </c>
       <c r="L7">
         <v>3</v>
@@ -18929,7 +19114,7 @@
       </c>
       <c r="C8">
         <f>AVERAGE(N:N)</f>
-        <v>1.8888888888888888</v>
+        <v>1.8181818181818181</v>
       </c>
       <c r="L8">
         <v>3</v>
@@ -18959,7 +19144,7 @@
       </c>
       <c r="C9">
         <f>5 - AVERAGE(P:P)</f>
-        <v>1.4444444444444446</v>
+        <v>1.4545454545454546</v>
       </c>
       <c r="L9">
         <v>3</v>
@@ -18989,7 +19174,7 @@
       </c>
       <c r="C10">
         <f>5 - AVERAGE(Q:Q)</f>
-        <v>1.3333333333333335</v>
+        <v>1.2727272727272729</v>
       </c>
       <c r="L10">
         <v>5</v>
@@ -19057,6 +19242,52 @@
       </c>
       <c r="R12">
         <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="L13">
+        <v>3</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>2</v>
+      </c>
+      <c r="O13">
+        <v>2</v>
+      </c>
+      <c r="P13">
+        <v>3</v>
+      </c>
+      <c r="Q13">
+        <v>4</v>
+      </c>
+      <c r="R13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <v>4</v>
+      </c>
+      <c r="Q14">
+        <v>4</v>
+      </c>
+      <c r="R14">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -19066,11 +19297,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:R12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="B4:R14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+      <selection activeCell="L13" sqref="L13:R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19081,7 +19312,7 @@
       </c>
       <c r="C4">
         <f>AVERAGE(L:L)</f>
-        <v>3.7777777777777777</v>
+        <v>3.9090909090909092</v>
       </c>
       <c r="L4">
         <v>5</v>
@@ -19111,7 +19342,7 @@
       </c>
       <c r="C5">
         <f>AVERAGE(O:O)</f>
-        <v>3.1111111111111112</v>
+        <v>3.1818181818181817</v>
       </c>
       <c r="L5">
         <v>4</v>
@@ -19141,7 +19372,7 @@
       </c>
       <c r="C6">
         <f>AVERAGE(M:M)</f>
-        <v>2.8888888888888888</v>
+        <v>3</v>
       </c>
       <c r="L6">
         <v>4</v>
@@ -19171,7 +19402,7 @@
       </c>
       <c r="C7">
         <f>5 - AVERAGE(R:R)</f>
-        <v>1.8888888888888888</v>
+        <v>1.9090909090909092</v>
       </c>
       <c r="L7">
         <v>3</v>
@@ -19201,7 +19432,7 @@
       </c>
       <c r="C8">
         <f>AVERAGE(N:N)</f>
-        <v>2.5555555555555554</v>
+        <v>2.5454545454545454</v>
       </c>
       <c r="L8">
         <v>3</v>
@@ -19231,7 +19462,7 @@
       </c>
       <c r="C9">
         <f>5 - AVERAGE(P:P)</f>
-        <v>2.1111111111111112</v>
+        <v>2.1818181818181817</v>
       </c>
       <c r="L9">
         <v>3</v>
@@ -19261,7 +19492,7 @@
       </c>
       <c r="C10">
         <f>5 - AVERAGE(Q:Q)</f>
-        <v>1.5555555555555554</v>
+        <v>1.7272727272727271</v>
       </c>
       <c r="L10">
         <v>4</v>
@@ -19329,6 +19560,52 @@
       </c>
       <c r="R12">
         <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="L13">
+        <v>4</v>
+      </c>
+      <c r="M13">
+        <v>3</v>
+      </c>
+      <c r="N13">
+        <v>2</v>
+      </c>
+      <c r="O13">
+        <v>3</v>
+      </c>
+      <c r="P13">
+        <v>3</v>
+      </c>
+      <c r="Q13">
+        <v>3</v>
+      </c>
+      <c r="R13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="L14">
+        <v>5</v>
+      </c>
+      <c r="M14">
+        <v>4</v>
+      </c>
+      <c r="N14">
+        <v>3</v>
+      </c>
+      <c r="O14">
+        <v>4</v>
+      </c>
+      <c r="P14">
+        <v>2</v>
+      </c>
+      <c r="Q14">
+        <v>2</v>
+      </c>
+      <c r="R14">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -19338,11 +19615,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:R12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="B4:R14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="L13" sqref="L13:R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19353,7 +19630,7 @@
       </c>
       <c r="C4">
         <f>AVERAGE(L:L)</f>
-        <v>3.6666666666666665</v>
+        <v>3.7272727272727271</v>
       </c>
       <c r="L4">
         <v>5</v>
@@ -19383,7 +19660,7 @@
       </c>
       <c r="C5">
         <f>AVERAGE(O:O)</f>
-        <v>3.2222222222222223</v>
+        <v>3.3636363636363638</v>
       </c>
       <c r="L5">
         <v>4</v>
@@ -19413,7 +19690,7 @@
       </c>
       <c r="C6">
         <f>AVERAGE(M:M)</f>
-        <v>3.4444444444444446</v>
+        <v>3.5454545454545454</v>
       </c>
       <c r="L6">
         <v>3</v>
@@ -19443,7 +19720,7 @@
       </c>
       <c r="C7">
         <f>5 - AVERAGE(R:R)</f>
-        <v>2.3333333333333335</v>
+        <v>2.2727272727272729</v>
       </c>
       <c r="L7">
         <v>3</v>
@@ -19473,7 +19750,7 @@
       </c>
       <c r="C8">
         <f>AVERAGE(N:N)</f>
-        <v>2.4444444444444446</v>
+        <v>2.4545454545454546</v>
       </c>
       <c r="L8">
         <v>4</v>
@@ -19503,7 +19780,7 @@
       </c>
       <c r="C9">
         <f>5 - AVERAGE(P:P)</f>
-        <v>2.1111111111111112</v>
+        <v>2.2727272727272729</v>
       </c>
       <c r="L9">
         <v>3</v>
@@ -19533,7 +19810,7 @@
       </c>
       <c r="C10">
         <f>5 - AVERAGE(Q:Q)</f>
-        <v>2</v>
+        <v>2.0909090909090908</v>
       </c>
       <c r="L10">
         <v>2</v>
@@ -19601,6 +19878,52 @@
       </c>
       <c r="R12">
         <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="L13">
+        <v>3</v>
+      </c>
+      <c r="M13">
+        <v>4</v>
+      </c>
+      <c r="N13">
+        <v>2</v>
+      </c>
+      <c r="O13">
+        <v>4</v>
+      </c>
+      <c r="P13">
+        <v>2</v>
+      </c>
+      <c r="Q13">
+        <v>3</v>
+      </c>
+      <c r="R13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="L14">
+        <v>5</v>
+      </c>
+      <c r="M14">
+        <v>4</v>
+      </c>
+      <c r="N14">
+        <v>3</v>
+      </c>
+      <c r="O14">
+        <v>4</v>
+      </c>
+      <c r="P14">
+        <v>2</v>
+      </c>
+      <c r="Q14">
+        <v>2</v>
+      </c>
+      <c r="R14">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -19610,11 +19933,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:R12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="B4:R14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C10"/>
+      <selection activeCell="L13" sqref="L13:R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19625,7 +19948,7 @@
       </c>
       <c r="C4">
         <f>AVERAGE(L:L)</f>
-        <v>3.3333333333333335</v>
+        <v>3.6363636363636362</v>
       </c>
       <c r="L4">
         <v>5</v>
@@ -19655,7 +19978,7 @@
       </c>
       <c r="C5">
         <f>AVERAGE(O:O)</f>
-        <v>2.6666666666666665</v>
+        <v>2.8181818181818183</v>
       </c>
       <c r="L5">
         <v>5</v>
@@ -19685,7 +20008,7 @@
       </c>
       <c r="C6">
         <f>AVERAGE(M:M)</f>
-        <v>2.7777777777777777</v>
+        <v>2.9090909090909092</v>
       </c>
       <c r="L6">
         <v>2</v>
@@ -19715,7 +20038,7 @@
       </c>
       <c r="C7">
         <f>5 - AVERAGE(R:R)</f>
-        <v>1.7777777777777777</v>
+        <v>1.8181818181818183</v>
       </c>
       <c r="L7">
         <v>2</v>
@@ -19745,7 +20068,7 @@
       </c>
       <c r="C8">
         <f>AVERAGE(N:N)</f>
-        <v>2.2222222222222223</v>
+        <v>2.1818181818181817</v>
       </c>
       <c r="L8">
         <v>3</v>
@@ -19775,7 +20098,7 @@
       </c>
       <c r="C9">
         <f>5 - AVERAGE(P:P)</f>
-        <v>2.1111111111111112</v>
+        <v>2.1818181818181817</v>
       </c>
       <c r="L9">
         <v>3</v>
@@ -19805,7 +20128,7 @@
       </c>
       <c r="C10">
         <f>5 - AVERAGE(Q:Q)</f>
-        <v>2.4444444444444446</v>
+        <v>2.4545454545454546</v>
       </c>
       <c r="L10">
         <v>4</v>
@@ -19873,6 +20196,52 @@
       </c>
       <c r="R12">
         <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="L13">
+        <v>5</v>
+      </c>
+      <c r="M13">
+        <v>4</v>
+      </c>
+      <c r="N13">
+        <v>2</v>
+      </c>
+      <c r="O13">
+        <v>3</v>
+      </c>
+      <c r="P13">
+        <v>3</v>
+      </c>
+      <c r="Q13">
+        <v>3</v>
+      </c>
+      <c r="R13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="L14">
+        <v>5</v>
+      </c>
+      <c r="M14">
+        <v>3</v>
+      </c>
+      <c r="N14">
+        <v>2</v>
+      </c>
+      <c r="O14">
+        <v>4</v>
+      </c>
+      <c r="P14">
+        <v>2</v>
+      </c>
+      <c r="Q14">
+        <v>2</v>
+      </c>
+      <c r="R14">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -19882,11 +20251,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:R12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="B4:R14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+      <selection activeCell="L13" sqref="L13:R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19897,7 +20266,7 @@
       </c>
       <c r="C4">
         <f>AVERAGE(L:L)</f>
-        <v>2.2222222222222223</v>
+        <v>2.0909090909090908</v>
       </c>
       <c r="L4">
         <v>3</v>
@@ -19927,7 +20296,7 @@
       </c>
       <c r="C5">
         <f>AVERAGE(O:O)</f>
-        <v>3.3333333333333335</v>
+        <v>3.2727272727272729</v>
       </c>
       <c r="L5">
         <v>3</v>
@@ -19957,7 +20326,7 @@
       </c>
       <c r="C6">
         <f>AVERAGE(M:M)</f>
-        <v>4</v>
+        <v>3.9090909090909092</v>
       </c>
       <c r="L6">
         <v>1</v>
@@ -19987,7 +20356,7 @@
       </c>
       <c r="C7">
         <f>5 - AVERAGE(R:R)</f>
-        <v>3.2222222222222223</v>
+        <v>3.0909090909090908</v>
       </c>
       <c r="L7">
         <v>1</v>
@@ -20017,7 +20386,7 @@
       </c>
       <c r="C8">
         <f>AVERAGE(N:N)</f>
-        <v>2.2222222222222223</v>
+        <v>2.2727272727272729</v>
       </c>
       <c r="L8">
         <v>2</v>
@@ -20047,7 +20416,7 @@
       </c>
       <c r="C9">
         <f>5 - AVERAGE(P:P)</f>
-        <v>2.4444444444444446</v>
+        <v>2.5454545454545454</v>
       </c>
       <c r="L9">
         <v>3</v>
@@ -20077,7 +20446,7 @@
       </c>
       <c r="C10">
         <f>5 - AVERAGE(Q:Q)</f>
-        <v>3</v>
+        <v>3.0909090909090908</v>
       </c>
       <c r="L10">
         <v>2</v>
@@ -20144,6 +20513,52 @@
         <v>4</v>
       </c>
       <c r="R12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="L13">
+        <v>2</v>
+      </c>
+      <c r="M13">
+        <v>5</v>
+      </c>
+      <c r="N13">
+        <v>4</v>
+      </c>
+      <c r="O13">
+        <v>4</v>
+      </c>
+      <c r="P13">
+        <v>2</v>
+      </c>
+      <c r="Q13">
+        <v>2</v>
+      </c>
+      <c r="R13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>2</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>2</v>
+      </c>
+      <c r="P14">
+        <v>2</v>
+      </c>
+      <c r="Q14">
+        <v>1</v>
+      </c>
+      <c r="R14">
         <v>2</v>
       </c>
     </row>
@@ -20154,11 +20569,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:R12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="B4:R14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C10"/>
+      <selection activeCell="L13" sqref="L13:R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20169,7 +20584,7 @@
       </c>
       <c r="C4">
         <f>AVERAGE(L:L)</f>
-        <v>4</v>
+        <v>3.9090909090909092</v>
       </c>
       <c r="L4">
         <v>5</v>
@@ -20199,7 +20614,7 @@
       </c>
       <c r="C5">
         <f>AVERAGE(O:O)</f>
-        <v>3.1111111111111112</v>
+        <v>3.1818181818181817</v>
       </c>
       <c r="L5">
         <v>4</v>
@@ -20229,7 +20644,7 @@
       </c>
       <c r="C6">
         <f>AVERAGE(M:M)</f>
-        <v>3.3333333333333335</v>
+        <v>3.2727272727272729</v>
       </c>
       <c r="L6">
         <v>4</v>
@@ -20259,7 +20674,7 @@
       </c>
       <c r="C7">
         <f>5 - AVERAGE(R:R)</f>
-        <v>2.25</v>
+        <v>2</v>
       </c>
       <c r="L7">
         <v>4</v>
@@ -20289,7 +20704,7 @@
       </c>
       <c r="C8">
         <f>AVERAGE(N:N)</f>
-        <v>1.6666666666666667</v>
+        <v>1.7272727272727273</v>
       </c>
       <c r="L8">
         <v>3</v>
@@ -20316,7 +20731,7 @@
       </c>
       <c r="C9">
         <f>5 - AVERAGE(P:P)</f>
-        <v>2.3333333333333335</v>
+        <v>2.2727272727272729</v>
       </c>
       <c r="L9">
         <v>3</v>
@@ -20346,7 +20761,7 @@
       </c>
       <c r="C10">
         <f>5 - AVERAGE(Q:Q)</f>
-        <v>2.1111111111111112</v>
+        <v>2.0909090909090908</v>
       </c>
       <c r="L10">
         <v>5</v>
@@ -20414,6 +20829,52 @@
       </c>
       <c r="R12">
         <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="L13">
+        <v>5</v>
+      </c>
+      <c r="M13">
+        <v>3</v>
+      </c>
+      <c r="N13">
+        <v>2</v>
+      </c>
+      <c r="O13">
+        <v>4</v>
+      </c>
+      <c r="P13">
+        <v>4</v>
+      </c>
+      <c r="Q13">
+        <v>3</v>
+      </c>
+      <c r="R13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="L14">
+        <v>2</v>
+      </c>
+      <c r="M14">
+        <v>3</v>
+      </c>
+      <c r="N14">
+        <v>2</v>
+      </c>
+      <c r="O14">
+        <v>3</v>
+      </c>
+      <c r="P14">
+        <v>2</v>
+      </c>
+      <c r="Q14">
+        <v>3</v>
+      </c>
+      <c r="R14">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -20423,11 +20884,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:R12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="B4:R14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+      <selection activeCell="L13" sqref="L13:R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20438,7 +20899,7 @@
       </c>
       <c r="C4">
         <f>AVERAGE(L:L)</f>
-        <v>3.7777777777777777</v>
+        <v>3.7272727272727271</v>
       </c>
       <c r="L4">
         <v>4</v>
@@ -20468,7 +20929,7 @@
       </c>
       <c r="C5">
         <f>AVERAGE(O:O)</f>
-        <v>3.4444444444444446</v>
+        <v>3.3636363636363638</v>
       </c>
       <c r="L5">
         <v>3</v>
@@ -20498,7 +20959,7 @@
       </c>
       <c r="C6">
         <f>AVERAGE(M:M)</f>
-        <v>3.2222222222222223</v>
+        <v>3.0909090909090908</v>
       </c>
       <c r="L6">
         <v>5</v>
@@ -20528,7 +20989,7 @@
       </c>
       <c r="C7">
         <f>5 - AVERAGE(R:R)</f>
-        <v>2.3333333333333335</v>
+        <v>2.4545454545454546</v>
       </c>
       <c r="L7">
         <v>3</v>
@@ -20558,7 +21019,7 @@
       </c>
       <c r="C8">
         <f>AVERAGE(N:N)</f>
-        <v>2.4444444444444446</v>
+        <v>2.4545454545454546</v>
       </c>
       <c r="L8">
         <v>3</v>
@@ -20588,7 +21049,7 @@
       </c>
       <c r="C9">
         <f>5 - AVERAGE(P:P)</f>
-        <v>2.1111111111111112</v>
+        <v>2.1818181818181817</v>
       </c>
       <c r="L9">
         <v>3</v>
@@ -20618,7 +21079,7 @@
       </c>
       <c r="C10">
         <f>5 - AVERAGE(Q:Q)</f>
-        <v>2.1111111111111112</v>
+        <v>2.1818181818181817</v>
       </c>
       <c r="L10">
         <v>4</v>
@@ -20685,6 +21146,52 @@
         <v>4</v>
       </c>
       <c r="R12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="L13">
+        <v>4</v>
+      </c>
+      <c r="M13">
+        <v>3</v>
+      </c>
+      <c r="N13">
+        <v>3</v>
+      </c>
+      <c r="O13">
+        <v>3</v>
+      </c>
+      <c r="P13">
+        <v>2</v>
+      </c>
+      <c r="Q13">
+        <v>3</v>
+      </c>
+      <c r="R13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="L14">
+        <v>3</v>
+      </c>
+      <c r="M14">
+        <v>2</v>
+      </c>
+      <c r="N14">
+        <v>2</v>
+      </c>
+      <c r="O14">
+        <v>3</v>
+      </c>
+      <c r="P14">
+        <v>3</v>
+      </c>
+      <c r="Q14">
+        <v>2</v>
+      </c>
+      <c r="R14">
         <v>2</v>
       </c>
     </row>
@@ -20695,11 +21202,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:R12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="B4:R14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C10"/>
+      <selection activeCell="L13" sqref="L13:R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20710,7 +21217,7 @@
       </c>
       <c r="C4">
         <f>AVERAGE(L:L)</f>
-        <v>3.4444444444444446</v>
+        <v>3.3636363636363638</v>
       </c>
       <c r="L4">
         <v>4</v>
@@ -20740,7 +21247,7 @@
       </c>
       <c r="C5">
         <f>AVERAGE(O:O)</f>
-        <v>3.2222222222222223</v>
+        <v>3.1818181818181817</v>
       </c>
       <c r="L5">
         <v>3</v>
@@ -20770,7 +21277,7 @@
       </c>
       <c r="C6">
         <f>AVERAGE(M:M)</f>
-        <v>3.5555555555555554</v>
+        <v>3.3636363636363638</v>
       </c>
       <c r="L6">
         <v>4</v>
@@ -20800,7 +21307,7 @@
       </c>
       <c r="C7">
         <f>5 - AVERAGE(R:R)</f>
-        <v>2.2222222222222223</v>
+        <v>2.1818181818181817</v>
       </c>
       <c r="L7">
         <v>3</v>
@@ -20830,7 +21337,7 @@
       </c>
       <c r="C8">
         <f>AVERAGE(N:N)</f>
-        <v>3.4444444444444446</v>
+        <v>3.4545454545454546</v>
       </c>
       <c r="L8">
         <v>3</v>
@@ -20860,7 +21367,7 @@
       </c>
       <c r="C9">
         <f>5 - AVERAGE(P:P)</f>
-        <v>1.3333333333333335</v>
+        <v>1.3636363636363638</v>
       </c>
       <c r="L9">
         <v>4</v>
@@ -20890,7 +21397,7 @@
       </c>
       <c r="C10">
         <f>5 - AVERAGE(Q:Q)</f>
-        <v>1.5555555555555554</v>
+        <v>1.7272727272727271</v>
       </c>
       <c r="L10">
         <v>3</v>
@@ -20957,6 +21464,52 @@
         <v>4</v>
       </c>
       <c r="R12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="L13">
+        <v>3</v>
+      </c>
+      <c r="M13">
+        <v>3</v>
+      </c>
+      <c r="N13">
+        <v>4</v>
+      </c>
+      <c r="O13">
+        <v>3</v>
+      </c>
+      <c r="P13">
+        <v>4</v>
+      </c>
+      <c r="Q13">
+        <v>3</v>
+      </c>
+      <c r="R13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="L14">
+        <v>3</v>
+      </c>
+      <c r="M14">
+        <v>2</v>
+      </c>
+      <c r="N14">
+        <v>3</v>
+      </c>
+      <c r="O14">
+        <v>3</v>
+      </c>
+      <c r="P14">
+        <v>3</v>
+      </c>
+      <c r="Q14">
+        <v>2</v>
+      </c>
+      <c r="R14">
         <v>2</v>
       </c>
     </row>

</xml_diff>